<commit_message>
added sounds into FMOD
</commit_message>
<xml_diff>
--- a/documentation/Asset List.xlsx
+++ b/documentation/Asset List.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexp\OneDrive\Desktop\671_final_project\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1E849F-A85A-4E65-9181-15419FC86B63}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-28920" yWindow="1620" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>Sound Name</t>
   </si>
@@ -107,62 +116,122 @@
   </si>
   <si>
     <t>Doors reached</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Disagree/sounds/433725/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/spycrah/sounds/471097/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/SoundFlakes/sounds/492239/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/qubodup/sounds/60027/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/dereklieu/sounds/241822/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/xpoki/sounds/432755/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Michel88/sounds/76959/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Aleks41/sounds/449552/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/238310/sounds/370189/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/Meisben/sounds/488037/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/JoelAudio/sounds/135463/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/cmorris035/sounds/319152/</t>
+  </si>
+  <si>
+    <t>https://freesound.org/people/FreqMan/sounds/23168/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
-    <font/>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  <cellStyleXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -352,25 +421,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.14"/>
-    <col customWidth="1" min="2" max="2" width="26.86"/>
-    <col customWidth="1" min="3" max="3" width="31.29"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="72" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -386,8 +461,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2">
+      <c r="F1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -404,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -420,8 +498,11 @@
       <c r="E3" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4">
+      <c r="F3" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>12</v>
       </c>
@@ -437,8 +518,11 @@
       <c r="E4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="5">
+      <c r="F4" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
@@ -454,8 +538,11 @@
       <c r="E5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6">
+      <c r="F5" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
@@ -471,8 +558,11 @@
       <c r="E6" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="7">
+      <c r="F6" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -488,8 +578,11 @@
       <c r="E7" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8">
+      <c r="F7" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -505,8 +598,11 @@
       <c r="E8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9">
+      <c r="F8" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -522,8 +618,11 @@
       <c r="E9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10">
+      <c r="F9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
@@ -539,8 +638,11 @@
       <c r="E10" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11">
+      <c r="F10" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>24</v>
       </c>
@@ -556,8 +658,11 @@
       <c r="E11" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="12">
+      <c r="F11" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -573,8 +678,11 @@
       <c r="E12" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13">
+      <c r="F12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>27</v>
       </c>
@@ -590,8 +698,11 @@
       <c r="E13" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14">
+      <c r="F13" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>28</v>
       </c>
@@ -607,8 +718,11 @@
       <c r="E14" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="15">
+      <c r="F14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -624,8 +738,11 @@
       <c r="E15" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="16">
+      <c r="F15" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>31</v>
       </c>
@@ -643,6 +760,21 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" xr:uid="{2517888B-A45C-4EBA-AAFF-B0D905783898}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{9C231CF0-C066-4319-81AF-57D8A95A89D7}"/>
+    <hyperlink ref="F5" r:id="rId3" xr:uid="{69108E37-3AC4-40D5-9C87-F98BA8FAD488}"/>
+    <hyperlink ref="F6" r:id="rId4" xr:uid="{85D50595-AB65-46E5-8B54-54AEF52E69B8}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{37B8DF20-BCF9-4FCB-ABE8-544077FF56FE}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{EF8E0B28-9477-4512-B790-0BB791DA5470}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{BE5C68AB-5DFC-439D-801C-E315247D6846}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{B728066B-0CC5-44BB-B424-0E976838AF99}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{4138FC77-20E9-4A1E-8795-38449F16DF67}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{0C26FB0D-61F3-4DBF-993C-BC30B6582A06}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{78CFDAF7-DDB3-4E3E-A13B-E3B59159F15A}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{B8A3CF18-42DB-40AF-8361-33EBEAC5C9BD}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{9A71FBAC-BF0A-4D55-A179-5709E9CD384F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>